<commit_message>
"Change Data with no attention"
</commit_message>
<xml_diff>
--- a/ResultProcess/BaseAndChange/txt_deal/all_excel/_sydney_bn_resnet_.xlsx
+++ b/ResultProcess/BaseAndChange/txt_deal/all_excel/_sydney_bn_resnet_.xlsx
@@ -416,25 +416,25 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.552</v>
+        <v>1.046</v>
       </c>
       <c r="D2" t="n">
-        <v>0.356</v>
+        <v>0.529</v>
       </c>
       <c r="E2" t="n">
-        <v>0.098</v>
+        <v>0.29</v>
       </c>
       <c r="F2" t="n">
-        <v>0.113</v>
+        <v>0.348</v>
       </c>
       <c r="G2" t="n">
-        <v>0.125</v>
+        <v>0.405</v>
       </c>
       <c r="H2" t="n">
-        <v>0.144</v>
+        <v>0.466</v>
       </c>
       <c r="I2" t="n">
-        <v>0.3405</v>
+        <v>0.5985</v>
       </c>
     </row>
     <row r="3">
@@ -445,25 +445,25 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>1.579</v>
+        <v>1.842</v>
       </c>
       <c r="D3" t="n">
-        <v>0.579</v>
+        <v>0.63</v>
       </c>
       <c r="E3" t="n">
-        <v>0.493</v>
+        <v>0.551</v>
       </c>
       <c r="F3" t="n">
-        <v>0.537</v>
+        <v>0.631</v>
       </c>
       <c r="G3" t="n">
-        <v>0.586</v>
+        <v>0.711</v>
       </c>
       <c r="H3" t="n">
-        <v>0.645</v>
+        <v>0.787</v>
       </c>
       <c r="I3" t="n">
-        <v>0.8075</v>
+        <v>0.91325</v>
       </c>
     </row>
     <row r="4">
@@ -474,25 +474,25 @@
         <v>10</v>
       </c>
       <c r="C4" t="n">
-        <v>2.03</v>
+        <v>2.311</v>
       </c>
       <c r="D4" t="n">
-        <v>0.665</v>
+        <v>0.71</v>
       </c>
       <c r="E4" t="n">
-        <v>0.551</v>
+        <v>0.57</v>
       </c>
       <c r="F4" t="n">
-        <v>0.629</v>
+        <v>0.648</v>
       </c>
       <c r="G4" t="n">
-        <v>0.71</v>
+        <v>0.728</v>
       </c>
       <c r="H4" t="n">
-        <v>0.794</v>
+        <v>0.804</v>
       </c>
       <c r="I4" t="n">
-        <v>0.97775</v>
+        <v>1.07525</v>
       </c>
     </row>
     <row r="5">
@@ -503,25 +503,25 @@
         <v>100</v>
       </c>
       <c r="C5" t="n">
-        <v>2.07</v>
+        <v>1.801</v>
       </c>
       <c r="D5" t="n">
-        <v>0.68</v>
+        <v>0.67</v>
       </c>
       <c r="E5" t="n">
-        <v>0.504</v>
+        <v>0.463</v>
       </c>
       <c r="F5" t="n">
-        <v>0.577</v>
+        <v>0.546</v>
       </c>
       <c r="G5" t="n">
-        <v>0.655</v>
+        <v>0.635</v>
       </c>
       <c r="H5" t="n">
-        <v>0.744</v>
+        <v>0.74</v>
       </c>
       <c r="I5" t="n">
-        <v>0.9835</v>
+        <v>0.901</v>
       </c>
     </row>
     <row r="6">
@@ -532,25 +532,25 @@
         <v>11</v>
       </c>
       <c r="C6" t="n">
-        <v>2.261</v>
+        <v>2.528</v>
       </c>
       <c r="D6" t="n">
-        <v>0.668</v>
+        <v>0.706</v>
       </c>
       <c r="E6" t="n">
-        <v>0.5649999999999999</v>
+        <v>0.588</v>
       </c>
       <c r="F6" t="n">
-        <v>0.643</v>
+        <v>0.657</v>
       </c>
       <c r="G6" t="n">
-        <v>0.721</v>
+        <v>0.727</v>
       </c>
       <c r="H6" t="n">
-        <v>0.801</v>
+        <v>0.8</v>
       </c>
       <c r="I6" t="n">
-        <v>1.0405</v>
+        <v>1.132</v>
       </c>
     </row>
     <row r="7">
@@ -561,25 +561,25 @@
         <v>12</v>
       </c>
       <c r="C7" t="n">
-        <v>2.13</v>
+        <v>2.67</v>
       </c>
       <c r="D7" t="n">
-        <v>0.675</v>
+        <v>0.727</v>
       </c>
       <c r="E7" t="n">
-        <v>0.538</v>
+        <v>0.605</v>
       </c>
       <c r="F7" t="n">
-        <v>0.613</v>
+        <v>0.676</v>
       </c>
       <c r="G7" t="n">
-        <v>0.6889999999999999</v>
+        <v>0.748</v>
       </c>
       <c r="H7" t="n">
-        <v>0.773</v>
+        <v>0.8169999999999999</v>
       </c>
       <c r="I7" t="n">
-        <v>1.0045</v>
+        <v>1.18225</v>
       </c>
     </row>
     <row r="8">
@@ -590,25 +590,25 @@
         <v>13</v>
       </c>
       <c r="C8" t="n">
-        <v>2.062</v>
+        <v>2.445</v>
       </c>
       <c r="D8" t="n">
-        <v>0.666</v>
+        <v>0.707</v>
       </c>
       <c r="E8" t="n">
-        <v>0.532</v>
+        <v>0.608</v>
       </c>
       <c r="F8" t="n">
-        <v>0.606</v>
+        <v>0.677</v>
       </c>
       <c r="G8" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.747</v>
       </c>
       <c r="H8" t="n">
-        <v>0.766</v>
+        <v>0.8159999999999999</v>
       </c>
       <c r="I8" t="n">
-        <v>0.9815</v>
+        <v>1.11675</v>
       </c>
     </row>
     <row r="9">
@@ -619,25 +619,25 @@
         <v>14</v>
       </c>
       <c r="C9" t="n">
-        <v>1.99</v>
+        <v>2.179</v>
       </c>
       <c r="D9" t="n">
-        <v>0.654</v>
+        <v>0.711</v>
       </c>
       <c r="E9" t="n">
-        <v>0.488</v>
+        <v>0.5669999999999999</v>
       </c>
       <c r="F9" t="n">
-        <v>0.571</v>
+        <v>0.646</v>
       </c>
       <c r="G9" t="n">
-        <v>0.654</v>
+        <v>0.728</v>
       </c>
       <c r="H9" t="n">
-        <v>0.739</v>
+        <v>0.806</v>
       </c>
       <c r="I9" t="n">
-        <v>0.9465</v>
+        <v>1.042</v>
       </c>
     </row>
     <row r="10">
@@ -648,25 +648,25 @@
         <v>15</v>
       </c>
       <c r="C10" t="n">
-        <v>1.947</v>
+        <v>2.328</v>
       </c>
       <c r="D10" t="n">
-        <v>0.656</v>
+        <v>0.705</v>
       </c>
       <c r="E10" t="n">
-        <v>0.529</v>
+        <v>0.595</v>
       </c>
       <c r="F10" t="n">
-        <v>0.611</v>
+        <v>0.66</v>
       </c>
       <c r="G10" t="n">
-        <v>0.6929999999999999</v>
+        <v>0.729</v>
       </c>
       <c r="H10" t="n">
-        <v>0.774</v>
+        <v>0.795</v>
       </c>
       <c r="I10" t="n">
-        <v>0.947</v>
+        <v>1.08325</v>
       </c>
     </row>
     <row r="11">
@@ -677,25 +677,25 @@
         <v>16</v>
       </c>
       <c r="C11" t="n">
-        <v>1.925</v>
+        <v>2.386</v>
       </c>
       <c r="D11" t="n">
-        <v>0.659</v>
+        <v>0.706</v>
       </c>
       <c r="E11" t="n">
-        <v>0.513</v>
+        <v>0.582</v>
       </c>
       <c r="F11" t="n">
-        <v>0.592</v>
+        <v>0.649</v>
       </c>
       <c r="G11" t="n">
-        <v>0.673</v>
+        <v>0.722</v>
       </c>
       <c r="H11" t="n">
-        <v>0.757</v>
+        <v>0.798</v>
       </c>
       <c r="I11" t="n">
-        <v>0.9389999999999999</v>
+        <v>1.095</v>
       </c>
     </row>
     <row r="12">
@@ -706,25 +706,25 @@
         <v>17</v>
       </c>
       <c r="C12" t="n">
-        <v>1.993</v>
+        <v>2.159</v>
       </c>
       <c r="D12" t="n">
-        <v>0.659</v>
+        <v>0.6889999999999999</v>
       </c>
       <c r="E12" t="n">
-        <v>0.524</v>
+        <v>0.523</v>
       </c>
       <c r="F12" t="n">
         <v>0.606</v>
       </c>
       <c r="G12" t="n">
-        <v>0.6860000000000001</v>
+        <v>0.6919999999999999</v>
       </c>
       <c r="H12" t="n">
-        <v>0.769</v>
+        <v>0.778</v>
       </c>
       <c r="I12" t="n">
-        <v>0.95875</v>
+        <v>1.015</v>
       </c>
     </row>
     <row r="13">
@@ -735,25 +735,25 @@
         <v>18</v>
       </c>
       <c r="C13" t="n">
-        <v>2.12</v>
+        <v>2.208</v>
       </c>
       <c r="D13" t="n">
-        <v>0.675</v>
+        <v>0.717</v>
       </c>
       <c r="E13" t="n">
-        <v>0.537</v>
+        <v>0.535</v>
       </c>
       <c r="F13" t="n">
-        <v>0.614</v>
+        <v>0.619</v>
       </c>
       <c r="G13" t="n">
-        <v>0.6929999999999999</v>
+        <v>0.707</v>
       </c>
       <c r="H13" t="n">
-        <v>0.777</v>
+        <v>0.792</v>
       </c>
       <c r="I13" t="n">
-        <v>1.00175</v>
+        <v>1.04425</v>
       </c>
     </row>
     <row r="14">
@@ -764,25 +764,25 @@
         <v>19</v>
       </c>
       <c r="C14" t="n">
-        <v>2.252</v>
+        <v>2.49</v>
       </c>
       <c r="D14" t="n">
-        <v>0.701</v>
+        <v>0.724</v>
       </c>
       <c r="E14" t="n">
-        <v>0.549</v>
+        <v>0.614</v>
       </c>
       <c r="F14" t="n">
-        <v>0.629</v>
+        <v>0.676</v>
       </c>
       <c r="G14" t="n">
-        <v>0.712</v>
+        <v>0.741</v>
       </c>
       <c r="H14" t="n">
-        <v>0.793</v>
+        <v>0.805</v>
       </c>
       <c r="I14" t="n">
-        <v>1.05075</v>
+        <v>1.138</v>
       </c>
     </row>
     <row r="15">
@@ -793,25 +793,25 @@
         <v>2</v>
       </c>
       <c r="C15" t="n">
-        <v>1.89</v>
+        <v>2.019</v>
       </c>
       <c r="D15" t="n">
-        <v>0.625</v>
+        <v>0.656</v>
       </c>
       <c r="E15" t="n">
-        <v>0.516</v>
+        <v>0.55</v>
       </c>
       <c r="F15" t="n">
-        <v>0.592</v>
+        <v>0.633</v>
       </c>
       <c r="G15" t="n">
-        <v>0.663</v>
+        <v>0.712</v>
       </c>
       <c r="H15" t="n">
-        <v>0.737</v>
+        <v>0.787</v>
       </c>
       <c r="I15" t="n">
-        <v>0.914</v>
+        <v>0.9702499999999999</v>
       </c>
     </row>
     <row r="16">
@@ -822,25 +822,25 @@
         <v>20</v>
       </c>
       <c r="C16" t="n">
-        <v>2.039</v>
+        <v>2.389</v>
       </c>
       <c r="D16" t="n">
-        <v>0.664</v>
+        <v>0.721</v>
       </c>
       <c r="E16" t="n">
-        <v>0.528</v>
+        <v>0.5620000000000001</v>
       </c>
       <c r="F16" t="n">
-        <v>0.609</v>
+        <v>0.638</v>
       </c>
       <c r="G16" t="n">
-        <v>0.6909999999999999</v>
+        <v>0.72</v>
       </c>
       <c r="H16" t="n">
-        <v>0.774</v>
+        <v>0.798</v>
       </c>
       <c r="I16" t="n">
-        <v>0.97375</v>
+        <v>1.09825</v>
       </c>
     </row>
     <row r="17">
@@ -851,25 +851,25 @@
         <v>21</v>
       </c>
       <c r="C17" t="n">
-        <v>2.057</v>
+        <v>1.98</v>
       </c>
       <c r="D17" t="n">
-        <v>0.676</v>
+        <v>0.677</v>
       </c>
       <c r="E17" t="n">
-        <v>0.503</v>
+        <v>0.532</v>
       </c>
       <c r="F17" t="n">
-        <v>0.592</v>
+        <v>0.607</v>
       </c>
       <c r="G17" t="n">
-        <v>0.677</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="H17" t="n">
-        <v>0.764</v>
+        <v>0.772</v>
       </c>
       <c r="I17" t="n">
-        <v>0.978</v>
+        <v>0.9665</v>
       </c>
     </row>
     <row r="18">
@@ -880,25 +880,25 @@
         <v>22</v>
       </c>
       <c r="C18" t="n">
-        <v>2.074</v>
+        <v>2.133</v>
       </c>
       <c r="D18" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.705</v>
       </c>
       <c r="E18" t="n">
-        <v>0.54</v>
+        <v>0.545</v>
       </c>
       <c r="F18" t="n">
-        <v>0.616</v>
+        <v>0.624</v>
       </c>
       <c r="G18" t="n">
-        <v>0.697</v>
+        <v>0.711</v>
       </c>
       <c r="H18" t="n">
-        <v>0.78</v>
+        <v>0.795</v>
       </c>
       <c r="I18" t="n">
-        <v>0.9985000000000001</v>
+        <v>1.022</v>
       </c>
     </row>
     <row r="19">
@@ -909,25 +909,25 @@
         <v>23</v>
       </c>
       <c r="C19" t="n">
-        <v>1.984</v>
+        <v>2.208</v>
       </c>
       <c r="D19" t="n">
-        <v>0.669</v>
+        <v>0.719</v>
       </c>
       <c r="E19" t="n">
-        <v>0.521</v>
+        <v>0.552</v>
       </c>
       <c r="F19" t="n">
-        <v>0.606</v>
+        <v>0.629</v>
       </c>
       <c r="G19" t="n">
-        <v>0.6919999999999999</v>
+        <v>0.71</v>
       </c>
       <c r="H19" t="n">
-        <v>0.778</v>
+        <v>0.787</v>
       </c>
       <c r="I19" t="n">
-        <v>0.96075</v>
+        <v>1.0495</v>
       </c>
     </row>
     <row r="20">
@@ -938,25 +938,25 @@
         <v>24</v>
       </c>
       <c r="C20" t="n">
-        <v>2.19</v>
+        <v>2.15</v>
       </c>
       <c r="D20" t="n">
-        <v>0.6909999999999999</v>
+        <v>0.698</v>
       </c>
       <c r="E20" t="n">
-        <v>0.534</v>
+        <v>0.547</v>
       </c>
       <c r="F20" t="n">
-        <v>0.612</v>
+        <v>0.631</v>
       </c>
       <c r="G20" t="n">
-        <v>0.696</v>
+        <v>0.718</v>
       </c>
       <c r="H20" t="n">
-        <v>0.783</v>
+        <v>0.799</v>
       </c>
       <c r="I20" t="n">
-        <v>1.0265</v>
+        <v>1.02325</v>
       </c>
     </row>
     <row r="21">
@@ -967,25 +967,25 @@
         <v>25</v>
       </c>
       <c r="C21" t="n">
-        <v>1.941</v>
+        <v>2.02</v>
       </c>
       <c r="D21" t="n">
-        <v>0.681</v>
+        <v>0.667</v>
       </c>
       <c r="E21" t="n">
-        <v>0.529</v>
+        <v>0.519</v>
       </c>
       <c r="F21" t="n">
-        <v>0.606</v>
+        <v>0.611</v>
       </c>
       <c r="G21" t="n">
-        <v>0.6909999999999999</v>
+        <v>0.703</v>
       </c>
       <c r="H21" t="n">
-        <v>0.776</v>
+        <v>0.791</v>
       </c>
       <c r="I21" t="n">
-        <v>0.958</v>
+        <v>0.9682500000000001</v>
       </c>
     </row>
     <row r="22">
@@ -996,25 +996,25 @@
         <v>26</v>
       </c>
       <c r="C22" t="n">
-        <v>2.174</v>
+        <v>2.31</v>
       </c>
       <c r="D22" t="n">
-        <v>0.696</v>
+        <v>0.719</v>
       </c>
       <c r="E22" t="n">
-        <v>0.532</v>
+        <v>0.54</v>
       </c>
       <c r="F22" t="n">
-        <v>0.61</v>
+        <v>0.622</v>
       </c>
       <c r="G22" t="n">
-        <v>0.6919999999999999</v>
+        <v>0.71</v>
       </c>
       <c r="H22" t="n">
-        <v>0.778</v>
+        <v>0.794</v>
       </c>
       <c r="I22" t="n">
-        <v>1.0245</v>
+        <v>1.072</v>
       </c>
     </row>
     <row r="23">
@@ -1025,25 +1025,25 @@
         <v>27</v>
       </c>
       <c r="C23" t="n">
-        <v>1.845</v>
+        <v>2.092</v>
       </c>
       <c r="D23" t="n">
-        <v>0.646</v>
+        <v>0.707</v>
       </c>
       <c r="E23" t="n">
-        <v>0.454</v>
+        <v>0.527</v>
       </c>
       <c r="F23" t="n">
-        <v>0.537</v>
+        <v>0.604</v>
       </c>
       <c r="G23" t="n">
-        <v>0.626</v>
+        <v>0.6889999999999999</v>
       </c>
       <c r="H23" t="n">
-        <v>0.726</v>
+        <v>0.773</v>
       </c>
       <c r="I23" t="n">
-        <v>0.89775</v>
+        <v>1.00825</v>
       </c>
     </row>
     <row r="24">
@@ -1054,25 +1054,25 @@
         <v>28</v>
       </c>
       <c r="C24" t="n">
-        <v>2.048</v>
+        <v>2.372</v>
       </c>
       <c r="D24" t="n">
-        <v>0.698</v>
+        <v>0.737</v>
       </c>
       <c r="E24" t="n">
-        <v>0.526</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="F24" t="n">
-        <v>0.605</v>
+        <v>0.638</v>
       </c>
       <c r="G24" t="n">
-        <v>0.6909999999999999</v>
+        <v>0.723</v>
       </c>
       <c r="H24" t="n">
-        <v>0.778</v>
+        <v>0.806</v>
       </c>
       <c r="I24" t="n">
-        <v>0.9925</v>
+        <v>1.1015</v>
       </c>
     </row>
     <row r="25">
@@ -1083,25 +1083,25 @@
         <v>29</v>
       </c>
       <c r="C25" t="n">
-        <v>2.058</v>
+        <v>2.159</v>
       </c>
       <c r="D25" t="n">
-        <v>0.71</v>
+        <v>0.715</v>
       </c>
       <c r="E25" t="n">
-        <v>0.541</v>
+        <v>0.571</v>
       </c>
       <c r="F25" t="n">
-        <v>0.621</v>
+        <v>0.64</v>
       </c>
       <c r="G25" t="n">
-        <v>0.704</v>
+        <v>0.716</v>
       </c>
       <c r="H25" t="n">
         <v>0.79</v>
       </c>
       <c r="I25" t="n">
-        <v>1.00475</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="26">
@@ -1112,25 +1112,25 @@
         <v>3</v>
       </c>
       <c r="C26" t="n">
-        <v>2.044</v>
+        <v>2.112</v>
       </c>
       <c r="D26" t="n">
-        <v>0.636</v>
+        <v>0.665</v>
       </c>
       <c r="E26" t="n">
-        <v>0.575</v>
+        <v>0.5659999999999999</v>
       </c>
       <c r="F26" t="n">
-        <v>0.646</v>
+        <v>0.64</v>
       </c>
       <c r="G26" t="n">
-        <v>0.71</v>
+        <v>0.715</v>
       </c>
       <c r="H26" t="n">
-        <v>0.776</v>
+        <v>0.785</v>
       </c>
       <c r="I26" t="n">
-        <v>0.97275</v>
+        <v>1.002</v>
       </c>
     </row>
     <row r="27">
@@ -1141,25 +1141,25 @@
         <v>30</v>
       </c>
       <c r="C27" t="n">
-        <v>1.853</v>
+        <v>2.125</v>
       </c>
       <c r="D27" t="n">
-        <v>0.663</v>
+        <v>0.695</v>
       </c>
       <c r="E27" t="n">
-        <v>0.468</v>
+        <v>0.533</v>
       </c>
       <c r="F27" t="n">
-        <v>0.549</v>
+        <v>0.613</v>
       </c>
       <c r="G27" t="n">
-        <v>0.639</v>
+        <v>0.701</v>
       </c>
       <c r="H27" t="n">
-        <v>0.741</v>
+        <v>0.788</v>
       </c>
       <c r="I27" t="n">
-        <v>0.9117499999999999</v>
+        <v>1.012</v>
       </c>
     </row>
     <row r="28">
@@ -1170,25 +1170,25 @@
         <v>31</v>
       </c>
       <c r="C28" t="n">
-        <v>1.944</v>
+        <v>2.215</v>
       </c>
       <c r="D28" t="n">
-        <v>0.6840000000000001</v>
+        <v>0.712</v>
       </c>
       <c r="E28" t="n">
-        <v>0.525</v>
+        <v>0.5659999999999999</v>
       </c>
       <c r="F28" t="n">
-        <v>0.602</v>
+        <v>0.641</v>
       </c>
       <c r="G28" t="n">
-        <v>0.6850000000000001</v>
+        <v>0.722</v>
       </c>
       <c r="H28" t="n">
-        <v>0.775</v>
+        <v>0.796</v>
       </c>
       <c r="I28" t="n">
-        <v>0.95925</v>
+        <v>1.05125</v>
       </c>
     </row>
     <row r="29">
@@ -1199,25 +1199,25 @@
         <v>32</v>
       </c>
       <c r="C29" t="n">
-        <v>1.944</v>
+        <v>2.334</v>
       </c>
       <c r="D29" t="n">
-        <v>0.6879999999999999</v>
+        <v>0.739</v>
       </c>
       <c r="E29" t="n">
-        <v>0.527</v>
+        <v>0.589</v>
       </c>
       <c r="F29" t="n">
-        <v>0.602</v>
+        <v>0.655</v>
       </c>
       <c r="G29" t="n">
-        <v>0.6860000000000001</v>
+        <v>0.728</v>
       </c>
       <c r="H29" t="n">
-        <v>0.771</v>
+        <v>0.799</v>
       </c>
       <c r="I29" t="n">
-        <v>0.96175</v>
+        <v>1.10025</v>
       </c>
     </row>
     <row r="30">
@@ -1228,25 +1228,25 @@
         <v>33</v>
       </c>
       <c r="C30" t="n">
-        <v>2.231</v>
+        <v>2.065</v>
       </c>
       <c r="D30" t="n">
-        <v>0.72</v>
+        <v>0.707</v>
       </c>
       <c r="E30" t="n">
-        <v>0.574</v>
+        <v>0.53</v>
       </c>
       <c r="F30" t="n">
-        <v>0.648</v>
+        <v>0.61</v>
       </c>
       <c r="G30" t="n">
-        <v>0.724</v>
+        <v>0.695</v>
       </c>
       <c r="H30" t="n">
-        <v>0.798</v>
+        <v>0.783</v>
       </c>
       <c r="I30" t="n">
-        <v>1.06125</v>
+        <v>1.00225</v>
       </c>
     </row>
     <row r="31">
@@ -1257,25 +1257,25 @@
         <v>34</v>
       </c>
       <c r="C31" t="n">
-        <v>2.211</v>
+        <v>1.914</v>
       </c>
       <c r="D31" t="n">
-        <v>0.714</v>
+        <v>0.68</v>
       </c>
       <c r="E31" t="n">
-        <v>0.5580000000000001</v>
+        <v>0.492</v>
       </c>
       <c r="F31" t="n">
-        <v>0.633</v>
+        <v>0.574</v>
       </c>
       <c r="G31" t="n">
-        <v>0.713</v>
+        <v>0.662</v>
       </c>
       <c r="H31" t="n">
-        <v>0.791</v>
+        <v>0.755</v>
       </c>
       <c r="I31" t="n">
-        <v>1.04925</v>
+        <v>0.9415</v>
       </c>
     </row>
     <row r="32">
@@ -1286,25 +1286,25 @@
         <v>35</v>
       </c>
       <c r="C32" t="n">
-        <v>1.851</v>
+        <v>2.029</v>
       </c>
       <c r="D32" t="n">
-        <v>0.662</v>
+        <v>0.701</v>
       </c>
       <c r="E32" t="n">
-        <v>0.483</v>
+        <v>0.519</v>
       </c>
       <c r="F32" t="n">
-        <v>0.5629999999999999</v>
+        <v>0.6</v>
       </c>
       <c r="G32" t="n">
-        <v>0.646</v>
+        <v>0.6860000000000001</v>
       </c>
       <c r="H32" t="n">
-        <v>0.74</v>
+        <v>0.769</v>
       </c>
       <c r="I32" t="n">
-        <v>0.9145</v>
+        <v>0.9875</v>
       </c>
     </row>
     <row r="33">
@@ -1315,25 +1315,25 @@
         <v>36</v>
       </c>
       <c r="C33" t="n">
-        <v>1.99</v>
+        <v>2.158</v>
       </c>
       <c r="D33" t="n">
-        <v>0.6929999999999999</v>
+        <v>0.718</v>
       </c>
       <c r="E33" t="n">
-        <v>0.534</v>
+        <v>0.575</v>
       </c>
       <c r="F33" t="n">
-        <v>0.614</v>
+        <v>0.644</v>
       </c>
       <c r="G33" t="n">
-        <v>0.697</v>
+        <v>0.721</v>
       </c>
       <c r="H33" t="n">
-        <v>0.781</v>
+        <v>0.8</v>
       </c>
       <c r="I33" t="n">
-        <v>0.9775</v>
+        <v>1.04225</v>
       </c>
     </row>
     <row r="34">
@@ -1344,25 +1344,25 @@
         <v>37</v>
       </c>
       <c r="C34" t="n">
-        <v>2.018</v>
+        <v>2.239</v>
       </c>
       <c r="D34" t="n">
-        <v>0.711</v>
+        <v>0.709</v>
       </c>
       <c r="E34" t="n">
-        <v>0.538</v>
+        <v>0.529</v>
       </c>
       <c r="F34" t="n">
-        <v>0.614</v>
+        <v>0.608</v>
       </c>
       <c r="G34" t="n">
-        <v>0.695</v>
+        <v>0.6929999999999999</v>
       </c>
       <c r="H34" t="n">
         <v>0.78</v>
       </c>
       <c r="I34" t="n">
-        <v>0.9945000000000001</v>
+        <v>1.0465</v>
       </c>
     </row>
     <row r="35">
@@ -1373,25 +1373,25 @@
         <v>38</v>
       </c>
       <c r="C35" t="n">
-        <v>1.96</v>
+        <v>2.297</v>
       </c>
       <c r="D35" t="n">
-        <v>0.6870000000000001</v>
+        <v>0.726</v>
       </c>
       <c r="E35" t="n">
-        <v>0.517</v>
+        <v>0.552</v>
       </c>
       <c r="F35" t="n">
-        <v>0.594</v>
+        <v>0.63</v>
       </c>
       <c r="G35" t="n">
-        <v>0.675</v>
+        <v>0.713</v>
       </c>
       <c r="H35" t="n">
-        <v>0.76</v>
+        <v>0.795</v>
       </c>
       <c r="I35" t="n">
-        <v>0.96275</v>
+        <v>1.07525</v>
       </c>
     </row>
     <row r="36">
@@ -1402,25 +1402,25 @@
         <v>39</v>
       </c>
       <c r="C36" t="n">
-        <v>1.798</v>
+        <v>2.302</v>
       </c>
       <c r="D36" t="n">
-        <v>0.677</v>
+        <v>0.734</v>
       </c>
       <c r="E36" t="n">
-        <v>0.49</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="F36" t="n">
-        <v>0.57</v>
+        <v>0.638</v>
       </c>
       <c r="G36" t="n">
-        <v>0.654</v>
+        <v>0.722</v>
       </c>
       <c r="H36" t="n">
-        <v>0.748</v>
+        <v>0.802</v>
       </c>
       <c r="I36" t="n">
-        <v>0.9105</v>
+        <v>1.0825</v>
       </c>
     </row>
     <row r="37">
@@ -1431,25 +1431,25 @@
         <v>4</v>
       </c>
       <c r="C37" t="n">
-        <v>2.001</v>
+        <v>2.357</v>
       </c>
       <c r="D37" t="n">
-        <v>0.644</v>
+        <v>0.6929999999999999</v>
       </c>
       <c r="E37" t="n">
-        <v>0.548</v>
+        <v>0.585</v>
       </c>
       <c r="F37" t="n">
-        <v>0.626</v>
+        <v>0.653</v>
       </c>
       <c r="G37" t="n">
-        <v>0.703</v>
+        <v>0.722</v>
       </c>
       <c r="H37" t="n">
-        <v>0.782</v>
+        <v>0.796</v>
       </c>
       <c r="I37" t="n">
-        <v>0.95925</v>
+        <v>1.082</v>
       </c>
     </row>
     <row r="38">
@@ -1460,25 +1460,25 @@
         <v>40</v>
       </c>
       <c r="C38" t="n">
-        <v>1.896</v>
+        <v>2.138</v>
       </c>
       <c r="D38" t="n">
-        <v>0.6889999999999999</v>
+        <v>0.719</v>
       </c>
       <c r="E38" t="n">
-        <v>0.542</v>
+        <v>0.527</v>
       </c>
       <c r="F38" t="n">
-        <v>0.622</v>
+        <v>0.61</v>
       </c>
       <c r="G38" t="n">
-        <v>0.706</v>
+        <v>0.696</v>
       </c>
       <c r="H38" t="n">
-        <v>0.79</v>
+        <v>0.783</v>
       </c>
       <c r="I38" t="n">
-        <v>0.954</v>
+        <v>1.02575</v>
       </c>
     </row>
     <row r="39">
@@ -1489,25 +1489,25 @@
         <v>41</v>
       </c>
       <c r="C39" t="n">
-        <v>2.14</v>
+        <v>2.195</v>
       </c>
       <c r="D39" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.724</v>
       </c>
       <c r="E39" t="n">
-        <v>0.513</v>
+        <v>0.5610000000000001</v>
       </c>
       <c r="F39" t="n">
-        <v>0.591</v>
+        <v>0.636</v>
       </c>
       <c r="G39" t="n">
-        <v>0.675</v>
+        <v>0.717</v>
       </c>
       <c r="H39" t="n">
-        <v>0.768</v>
+        <v>0.797</v>
       </c>
       <c r="I39" t="n">
-        <v>1.00825</v>
+        <v>1.051</v>
       </c>
     </row>
     <row r="40">
@@ -1518,25 +1518,25 @@
         <v>42</v>
       </c>
       <c r="C40" t="n">
-        <v>1.943</v>
+        <v>2.066</v>
       </c>
       <c r="D40" t="n">
-        <v>0.6840000000000001</v>
+        <v>0.711</v>
       </c>
       <c r="E40" t="n">
-        <v>0.512</v>
+        <v>0.543</v>
       </c>
       <c r="F40" t="n">
-        <v>0.588</v>
+        <v>0.623</v>
       </c>
       <c r="G40" t="n">
-        <v>0.672</v>
+        <v>0.706</v>
       </c>
       <c r="H40" t="n">
-        <v>0.762</v>
+        <v>0.79</v>
       </c>
       <c r="I40" t="n">
-        <v>0.95575</v>
+        <v>1.00775</v>
       </c>
     </row>
     <row r="41">
@@ -1547,25 +1547,25 @@
         <v>43</v>
       </c>
       <c r="C41" t="n">
-        <v>2.053</v>
+        <v>2.171</v>
       </c>
       <c r="D41" t="n">
-        <v>0.694</v>
+        <v>0.722</v>
       </c>
       <c r="E41" t="n">
-        <v>0.522</v>
+        <v>0.541</v>
       </c>
       <c r="F41" t="n">
-        <v>0.598</v>
+        <v>0.617</v>
       </c>
       <c r="G41" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.699</v>
       </c>
       <c r="H41" t="n">
-        <v>0.771</v>
+        <v>0.787</v>
       </c>
       <c r="I41" t="n">
-        <v>0.99075</v>
+        <v>1.039</v>
       </c>
     </row>
     <row r="42">
@@ -1576,25 +1576,25 @@
         <v>44</v>
       </c>
       <c r="C42" t="n">
-        <v>2.041</v>
+        <v>2.168</v>
       </c>
       <c r="D42" t="n">
-        <v>0.699</v>
+        <v>0.706</v>
       </c>
       <c r="E42" t="n">
-        <v>0.507</v>
+        <v>0.528</v>
       </c>
       <c r="F42" t="n">
-        <v>0.583</v>
+        <v>0.607</v>
       </c>
       <c r="G42" t="n">
-        <v>0.666</v>
+        <v>0.6929999999999999</v>
       </c>
       <c r="H42" t="n">
-        <v>0.76</v>
+        <v>0.781</v>
       </c>
       <c r="I42" t="n">
-        <v>0.9865</v>
+        <v>1.027</v>
       </c>
     </row>
     <row r="43">
@@ -1605,25 +1605,25 @@
         <v>45</v>
       </c>
       <c r="C43" t="n">
-        <v>1.933</v>
+        <v>2.016</v>
       </c>
       <c r="D43" t="n">
-        <v>0.696</v>
+        <v>0.6909999999999999</v>
       </c>
       <c r="E43" t="n">
-        <v>0.526</v>
+        <v>0.505</v>
       </c>
       <c r="F43" t="n">
-        <v>0.602</v>
+        <v>0.582</v>
       </c>
       <c r="G43" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.665</v>
       </c>
       <c r="H43" t="n">
-        <v>0.771</v>
+        <v>0.757</v>
       </c>
       <c r="I43" t="n">
-        <v>0.96275</v>
+        <v>0.97575</v>
       </c>
     </row>
     <row r="44">
@@ -1634,25 +1634,25 @@
         <v>46</v>
       </c>
       <c r="C44" t="n">
-        <v>2.253</v>
+        <v>2.357</v>
       </c>
       <c r="D44" t="n">
-        <v>0.717</v>
+        <v>0.736</v>
       </c>
       <c r="E44" t="n">
-        <v>0.538</v>
+        <v>0.554</v>
       </c>
       <c r="F44" t="n">
-        <v>0.619</v>
+        <v>0.634</v>
       </c>
       <c r="G44" t="n">
-        <v>0.703</v>
+        <v>0.72</v>
       </c>
       <c r="H44" t="n">
-        <v>0.783</v>
+        <v>0.805</v>
       </c>
       <c r="I44" t="n">
-        <v>1.05625</v>
+        <v>1.09575</v>
       </c>
     </row>
     <row r="45">
@@ -1663,25 +1663,25 @@
         <v>47</v>
       </c>
       <c r="C45" t="n">
-        <v>1.933</v>
+        <v>2.169</v>
       </c>
       <c r="D45" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.708</v>
       </c>
       <c r="E45" t="n">
-        <v>0.512</v>
+        <v>0.547</v>
       </c>
       <c r="F45" t="n">
-        <v>0.585</v>
+        <v>0.624</v>
       </c>
       <c r="G45" t="n">
-        <v>0.665</v>
+        <v>0.706</v>
       </c>
       <c r="H45" t="n">
-        <v>0.755</v>
+        <v>0.789</v>
       </c>
       <c r="I45" t="n">
-        <v>0.95275</v>
+        <v>1.033</v>
       </c>
     </row>
     <row r="46">
@@ -1692,25 +1692,25 @@
         <v>48</v>
       </c>
       <c r="C46" t="n">
-        <v>1.865</v>
+        <v>1.98</v>
       </c>
       <c r="D46" t="n">
-        <v>0.661</v>
+        <v>0.6840000000000001</v>
       </c>
       <c r="E46" t="n">
-        <v>0.501</v>
+        <v>0.493</v>
       </c>
       <c r="F46" t="n">
-        <v>0.582</v>
+        <v>0.577</v>
       </c>
       <c r="G46" t="n">
-        <v>0.666</v>
+        <v>0.665</v>
       </c>
       <c r="H46" t="n">
-        <v>0.757</v>
+        <v>0.759</v>
       </c>
       <c r="I46" t="n">
-        <v>0.922</v>
+        <v>0.96025</v>
       </c>
     </row>
     <row r="47">
@@ -1721,25 +1721,25 @@
         <v>49</v>
       </c>
       <c r="C47" t="n">
-        <v>1.896</v>
+        <v>2.003</v>
       </c>
       <c r="D47" t="n">
-        <v>0.656</v>
+        <v>0.697</v>
       </c>
       <c r="E47" t="n">
-        <v>0.454</v>
+        <v>0.531</v>
       </c>
       <c r="F47" t="n">
-        <v>0.535</v>
+        <v>0.608</v>
       </c>
       <c r="G47" t="n">
-        <v>0.624</v>
+        <v>0.6889999999999999</v>
       </c>
       <c r="H47" t="n">
-        <v>0.727</v>
+        <v>0.774</v>
       </c>
       <c r="I47" t="n">
-        <v>0.9155</v>
+        <v>0.982</v>
       </c>
     </row>
     <row r="48">
@@ -1750,25 +1750,25 @@
         <v>5</v>
       </c>
       <c r="C48" t="n">
-        <v>2.076</v>
+        <v>2.533</v>
       </c>
       <c r="D48" t="n">
-        <v>0.649</v>
+        <v>0.699</v>
       </c>
       <c r="E48" t="n">
-        <v>0.538</v>
+        <v>0.586</v>
       </c>
       <c r="F48" t="n">
-        <v>0.614</v>
+        <v>0.658</v>
       </c>
       <c r="G48" t="n">
-        <v>0.6929999999999999</v>
+        <v>0.732</v>
       </c>
       <c r="H48" t="n">
-        <v>0.778</v>
+        <v>0.805</v>
       </c>
       <c r="I48" t="n">
-        <v>0.978</v>
+        <v>1.12925</v>
       </c>
     </row>
     <row r="49">
@@ -1779,25 +1779,25 @@
         <v>50</v>
       </c>
       <c r="C49" t="n">
-        <v>1.723</v>
+        <v>2.062</v>
       </c>
       <c r="D49" t="n">
-        <v>0.631</v>
+        <v>0.695</v>
       </c>
       <c r="E49" t="n">
-        <v>0.452</v>
+        <v>0.533</v>
       </c>
       <c r="F49" t="n">
-        <v>0.53</v>
+        <v>0.612</v>
       </c>
       <c r="G49" t="n">
-        <v>0.613</v>
+        <v>0.694</v>
       </c>
       <c r="H49" t="n">
-        <v>0.713</v>
+        <v>0.776</v>
       </c>
       <c r="I49" t="n">
-        <v>0.85925</v>
+        <v>0.99625</v>
       </c>
     </row>
     <row r="50">
@@ -1808,25 +1808,25 @@
         <v>51</v>
       </c>
       <c r="C50" t="n">
-        <v>2.102</v>
+        <v>2.089</v>
       </c>
       <c r="D50" t="n">
-        <v>0.6830000000000001</v>
+        <v>0.697</v>
       </c>
       <c r="E50" t="n">
-        <v>0.498</v>
+        <v>0.525</v>
       </c>
       <c r="F50" t="n">
-        <v>0.575</v>
+        <v>0.605</v>
       </c>
       <c r="G50" t="n">
-        <v>0.657</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="H50" t="n">
-        <v>0.751</v>
+        <v>0.778</v>
       </c>
       <c r="I50" t="n">
-        <v>0.9915</v>
+        <v>1.002</v>
       </c>
     </row>
     <row r="51">
@@ -1837,25 +1837,25 @@
         <v>52</v>
       </c>
       <c r="C51" t="n">
-        <v>1.955</v>
+        <v>1.952</v>
       </c>
       <c r="D51" t="n">
-        <v>0.672</v>
+        <v>0.6879999999999999</v>
       </c>
       <c r="E51" t="n">
-        <v>0.473</v>
+        <v>0.48</v>
       </c>
       <c r="F51" t="n">
-        <v>0.553</v>
+        <v>0.5629999999999999</v>
       </c>
       <c r="G51" t="n">
-        <v>0.637</v>
+        <v>0.651</v>
       </c>
       <c r="H51" t="n">
-        <v>0.733</v>
+        <v>0.751</v>
       </c>
       <c r="I51" t="n">
-        <v>0.9429999999999999</v>
+        <v>0.952</v>
       </c>
     </row>
     <row r="52">
@@ -1866,25 +1866,25 @@
         <v>53</v>
       </c>
       <c r="C52" t="n">
-        <v>1.719</v>
+        <v>2.025</v>
       </c>
       <c r="D52" t="n">
-        <v>0.645</v>
+        <v>0.673</v>
       </c>
       <c r="E52" t="n">
-        <v>0.46</v>
+        <v>0.468</v>
       </c>
       <c r="F52" t="n">
-        <v>0.545</v>
+        <v>0.5570000000000001</v>
       </c>
       <c r="G52" t="n">
-        <v>0.633</v>
+        <v>0.648</v>
       </c>
       <c r="H52" t="n">
-        <v>0.738</v>
+        <v>0.749</v>
       </c>
       <c r="I52" t="n">
-        <v>0.86725</v>
+        <v>0.95975</v>
       </c>
     </row>
     <row r="53">
@@ -1895,25 +1895,25 @@
         <v>54</v>
       </c>
       <c r="C53" t="n">
-        <v>2.08</v>
+        <v>2.136</v>
       </c>
       <c r="D53" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.712</v>
       </c>
       <c r="E53" t="n">
-        <v>0.501</v>
+        <v>0.532</v>
       </c>
       <c r="F53" t="n">
-        <v>0.58</v>
+        <v>0.607</v>
       </c>
       <c r="G53" t="n">
-        <v>0.662</v>
+        <v>0.6879999999999999</v>
       </c>
       <c r="H53" t="n">
-        <v>0.755</v>
+        <v>0.775</v>
       </c>
       <c r="I53" t="n">
-        <v>0.99025</v>
+        <v>1.023</v>
       </c>
     </row>
     <row r="54">
@@ -1924,25 +1924,25 @@
         <v>55</v>
       </c>
       <c r="C54" t="n">
-        <v>2.005</v>
+        <v>2.12</v>
       </c>
       <c r="D54" t="n">
-        <v>0.6870000000000001</v>
+        <v>0.703</v>
       </c>
       <c r="E54" t="n">
-        <v>0.521</v>
+        <v>0.529</v>
       </c>
       <c r="F54" t="n">
-        <v>0.597</v>
+        <v>0.608</v>
       </c>
       <c r="G54" t="n">
-        <v>0.676</v>
+        <v>0.6929999999999999</v>
       </c>
       <c r="H54" t="n">
-        <v>0.763</v>
+        <v>0.778</v>
       </c>
       <c r="I54" t="n">
-        <v>0.975</v>
+        <v>1.01375</v>
       </c>
     </row>
     <row r="55">
@@ -1953,25 +1953,25 @@
         <v>56</v>
       </c>
       <c r="C55" t="n">
-        <v>1.956</v>
+        <v>2.147</v>
       </c>
       <c r="D55" t="n">
-        <v>0.639</v>
+        <v>0.714</v>
       </c>
       <c r="E55" t="n">
-        <v>0.458</v>
+        <v>0.542</v>
       </c>
       <c r="F55" t="n">
-        <v>0.536</v>
+        <v>0.62</v>
       </c>
       <c r="G55" t="n">
-        <v>0.62</v>
+        <v>0.704</v>
       </c>
       <c r="H55" t="n">
-        <v>0.722</v>
+        <v>0.788</v>
       </c>
       <c r="I55" t="n">
-        <v>0.923</v>
+        <v>1.02925</v>
       </c>
     </row>
     <row r="56">
@@ -1982,25 +1982,25 @@
         <v>57</v>
       </c>
       <c r="C56" t="n">
-        <v>1.924</v>
+        <v>1.996</v>
       </c>
       <c r="D56" t="n">
-        <v>0.651</v>
+        <v>0.703</v>
       </c>
       <c r="E56" t="n">
-        <v>0.466</v>
+        <v>0.541</v>
       </c>
       <c r="F56" t="n">
-        <v>0.541</v>
+        <v>0.624</v>
       </c>
       <c r="G56" t="n">
-        <v>0.624</v>
+        <v>0.706</v>
       </c>
       <c r="H56" t="n">
-        <v>0.722</v>
+        <v>0.785</v>
       </c>
       <c r="I56" t="n">
-        <v>0.923</v>
+        <v>0.98575</v>
       </c>
     </row>
     <row r="57">
@@ -2011,25 +2011,25 @@
         <v>58</v>
       </c>
       <c r="C57" t="n">
-        <v>1.95</v>
+        <v>2.183</v>
       </c>
       <c r="D57" t="n">
-        <v>0.678</v>
+        <v>0.707</v>
       </c>
       <c r="E57" t="n">
-        <v>0.508</v>
+        <v>0.536</v>
       </c>
       <c r="F57" t="n">
-        <v>0.583</v>
+        <v>0.614</v>
       </c>
       <c r="G57" t="n">
-        <v>0.664</v>
+        <v>0.694</v>
       </c>
       <c r="H57" t="n">
-        <v>0.757</v>
+        <v>0.778</v>
       </c>
       <c r="I57" t="n">
-        <v>0.9535</v>
+        <v>1.03325</v>
       </c>
     </row>
     <row r="58">
@@ -2040,25 +2040,25 @@
         <v>59</v>
       </c>
       <c r="C58" t="n">
-        <v>1.913</v>
+        <v>2.072</v>
       </c>
       <c r="D58" t="n">
-        <v>0.673</v>
+        <v>0.701</v>
       </c>
       <c r="E58" t="n">
-        <v>0.503</v>
+        <v>0.532</v>
       </c>
       <c r="F58" t="n">
-        <v>0.579</v>
+        <v>0.608</v>
       </c>
       <c r="G58" t="n">
-        <v>0.661</v>
+        <v>0.6879999999999999</v>
       </c>
       <c r="H58" t="n">
-        <v>0.753</v>
+        <v>0.776</v>
       </c>
       <c r="I58" t="n">
-        <v>0.9405</v>
+        <v>1.0015</v>
       </c>
     </row>
     <row r="59">
@@ -2069,25 +2069,25 @@
         <v>6</v>
       </c>
       <c r="C59" t="n">
-        <v>2.095</v>
+        <v>2.306</v>
       </c>
       <c r="D59" t="n">
-        <v>0.668</v>
+        <v>0.6860000000000001</v>
       </c>
       <c r="E59" t="n">
-        <v>0.5620000000000001</v>
+        <v>0.556</v>
       </c>
       <c r="F59" t="n">
-        <v>0.641</v>
+        <v>0.632</v>
       </c>
       <c r="G59" t="n">
-        <v>0.723</v>
+        <v>0.71</v>
       </c>
       <c r="H59" t="n">
-        <v>0.804</v>
+        <v>0.795</v>
       </c>
       <c r="I59" t="n">
-        <v>0.99825</v>
+        <v>1.0585</v>
       </c>
     </row>
     <row r="60">
@@ -2098,25 +2098,25 @@
         <v>60</v>
       </c>
       <c r="C60" t="n">
-        <v>1.985</v>
+        <v>1.975</v>
       </c>
       <c r="D60" t="n">
-        <v>0.669</v>
+        <v>0.714</v>
       </c>
       <c r="E60" t="n">
-        <v>0.515</v>
+        <v>0.544</v>
       </c>
       <c r="F60" t="n">
-        <v>0.59</v>
+        <v>0.616</v>
       </c>
       <c r="G60" t="n">
-        <v>0.669</v>
+        <v>0.696</v>
       </c>
       <c r="H60" t="n">
-        <v>0.757</v>
+        <v>0.781</v>
       </c>
       <c r="I60" t="n">
-        <v>0.9595</v>
+        <v>0.98675</v>
       </c>
     </row>
     <row r="61">
@@ -2127,25 +2127,25 @@
         <v>61</v>
       </c>
       <c r="C61" t="n">
-        <v>1.922</v>
+        <v>2.197</v>
       </c>
       <c r="D61" t="n">
-        <v>0.674</v>
+        <v>0.6929999999999999</v>
       </c>
       <c r="E61" t="n">
-        <v>0.474</v>
+        <v>0.582</v>
       </c>
       <c r="F61" t="n">
-        <v>0.555</v>
+        <v>0.647</v>
       </c>
       <c r="G61" t="n">
-        <v>0.641</v>
+        <v>0.718</v>
       </c>
       <c r="H61" t="n">
-        <v>0.737</v>
+        <v>0.793</v>
       </c>
       <c r="I61" t="n">
-        <v>0.9360000000000001</v>
+        <v>1.04125</v>
       </c>
     </row>
     <row r="62">
@@ -2156,25 +2156,25 @@
         <v>62</v>
       </c>
       <c r="C62" t="n">
-        <v>1.959</v>
+        <v>1.838</v>
       </c>
       <c r="D62" t="n">
-        <v>0.6820000000000001</v>
+        <v>0.676</v>
       </c>
       <c r="E62" t="n">
-        <v>0.515</v>
+        <v>0.499</v>
       </c>
       <c r="F62" t="n">
-        <v>0.592</v>
+        <v>0.578</v>
       </c>
       <c r="G62" t="n">
-        <v>0.674</v>
+        <v>0.662</v>
       </c>
       <c r="H62" t="n">
-        <v>0.769</v>
+        <v>0.752</v>
       </c>
       <c r="I62" t="n">
-        <v>0.9595</v>
+        <v>0.92225</v>
       </c>
     </row>
     <row r="63">
@@ -2185,25 +2185,25 @@
         <v>63</v>
       </c>
       <c r="C63" t="n">
-        <v>2.094</v>
+        <v>2.216</v>
       </c>
       <c r="D63" t="n">
-        <v>0.6909999999999999</v>
+        <v>0.725</v>
       </c>
       <c r="E63" t="n">
-        <v>0.485</v>
+        <v>0.552</v>
       </c>
       <c r="F63" t="n">
-        <v>0.5679999999999999</v>
+        <v>0.633</v>
       </c>
       <c r="G63" t="n">
-        <v>0.656</v>
+        <v>0.72</v>
       </c>
       <c r="H63" t="n">
-        <v>0.755</v>
+        <v>0.803</v>
       </c>
       <c r="I63" t="n">
-        <v>0.99025</v>
+        <v>1.0545</v>
       </c>
     </row>
     <row r="64">
@@ -2214,25 +2214,25 @@
         <v>64</v>
       </c>
       <c r="C64" t="n">
-        <v>2.142</v>
+        <v>1.933</v>
       </c>
       <c r="D64" t="n">
-        <v>0.6929999999999999</v>
+        <v>0.678</v>
       </c>
       <c r="E64" t="n">
-        <v>0.5649999999999999</v>
+        <v>0.481</v>
       </c>
       <c r="F64" t="n">
-        <v>0.643</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="G64" t="n">
-        <v>0.721</v>
+        <v>0.646</v>
       </c>
       <c r="H64" t="n">
-        <v>0.802</v>
+        <v>0.746</v>
       </c>
       <c r="I64" t="n">
-        <v>1.02325</v>
+        <v>0.9425</v>
       </c>
     </row>
     <row r="65">
@@ -2243,25 +2243,25 @@
         <v>65</v>
       </c>
       <c r="C65" t="n">
-        <v>1.984</v>
+        <v>1.85</v>
       </c>
       <c r="D65" t="n">
-        <v>0.675</v>
+        <v>0.678</v>
       </c>
       <c r="E65" t="n">
-        <v>0.487</v>
+        <v>0.496</v>
       </c>
       <c r="F65" t="n">
-        <v>0.5669999999999999</v>
+        <v>0.574</v>
       </c>
       <c r="G65" t="n">
-        <v>0.65</v>
+        <v>0.659</v>
       </c>
       <c r="H65" t="n">
-        <v>0.746</v>
+        <v>0.753</v>
       </c>
       <c r="I65" t="n">
-        <v>0.95525</v>
+        <v>0.9255</v>
       </c>
     </row>
     <row r="66">
@@ -2272,25 +2272,25 @@
         <v>66</v>
       </c>
       <c r="C66" t="n">
-        <v>1.878</v>
+        <v>2.11</v>
       </c>
       <c r="D66" t="n">
-        <v>0.655</v>
+        <v>0.701</v>
       </c>
       <c r="E66" t="n">
-        <v>0.467</v>
+        <v>0.5570000000000001</v>
       </c>
       <c r="F66" t="n">
-        <v>0.551</v>
+        <v>0.629</v>
       </c>
       <c r="G66" t="n">
-        <v>0.639</v>
+        <v>0.707</v>
       </c>
       <c r="H66" t="n">
-        <v>0.735</v>
+        <v>0.794</v>
       </c>
       <c r="I66" t="n">
-        <v>0.91375</v>
+        <v>1.01725</v>
       </c>
     </row>
     <row r="67">
@@ -2301,25 +2301,25 @@
         <v>67</v>
       </c>
       <c r="C67" t="n">
-        <v>2.112</v>
+        <v>2.023</v>
       </c>
       <c r="D67" t="n">
-        <v>0.699</v>
+        <v>0.696</v>
       </c>
       <c r="E67" t="n">
-        <v>0.548</v>
+        <v>0.522</v>
       </c>
       <c r="F67" t="n">
-        <v>0.622</v>
+        <v>0.604</v>
       </c>
       <c r="G67" t="n">
-        <v>0.7</v>
+        <v>0.6929999999999999</v>
       </c>
       <c r="H67" t="n">
-        <v>0.787</v>
+        <v>0.782</v>
       </c>
       <c r="I67" t="n">
-        <v>1.0145</v>
+        <v>0.98425</v>
       </c>
     </row>
     <row r="68">
@@ -2330,25 +2330,25 @@
         <v>68</v>
       </c>
       <c r="C68" t="n">
-        <v>2.073</v>
+        <v>2.057</v>
       </c>
       <c r="D68" t="n">
-        <v>0.675</v>
+        <v>0.704</v>
       </c>
       <c r="E68" t="n">
-        <v>0.477</v>
+        <v>0.532</v>
       </c>
       <c r="F68" t="n">
-        <v>0.553</v>
+        <v>0.613</v>
       </c>
       <c r="G68" t="n">
-        <v>0.634</v>
+        <v>0.7</v>
       </c>
       <c r="H68" t="n">
-        <v>0.733</v>
+        <v>0.789</v>
       </c>
       <c r="I68" t="n">
-        <v>0.975</v>
+        <v>0.99925</v>
       </c>
     </row>
     <row r="69">
@@ -2359,25 +2359,25 @@
         <v>69</v>
       </c>
       <c r="C69" t="n">
-        <v>2.042</v>
+        <v>1.966</v>
       </c>
       <c r="D69" t="n">
-        <v>0.662</v>
+        <v>0.6840000000000001</v>
       </c>
       <c r="E69" t="n">
-        <v>0.512</v>
+        <v>0.522</v>
       </c>
       <c r="F69" t="n">
-        <v>0.591</v>
+        <v>0.599</v>
       </c>
       <c r="G69" t="n">
-        <v>0.672</v>
+        <v>0.681</v>
       </c>
       <c r="H69" t="n">
-        <v>0.758</v>
+        <v>0.769</v>
       </c>
       <c r="I69" t="n">
-        <v>0.9695</v>
+        <v>0.964</v>
       </c>
     </row>
     <row r="70">
@@ -2388,25 +2388,25 @@
         <v>7</v>
       </c>
       <c r="C70" t="n">
-        <v>2.114</v>
+        <v>2.657</v>
       </c>
       <c r="D70" t="n">
-        <v>0.666</v>
+        <v>0.719</v>
       </c>
       <c r="E70" t="n">
-        <v>0.55</v>
+        <v>0.604</v>
       </c>
       <c r="F70" t="n">
-        <v>0.629</v>
+        <v>0.673</v>
       </c>
       <c r="G70" t="n">
-        <v>0.706</v>
+        <v>0.746</v>
       </c>
       <c r="H70" t="n">
-        <v>0.789</v>
+        <v>0.825</v>
       </c>
       <c r="I70" t="n">
-        <v>0.999</v>
+        <v>1.17475</v>
       </c>
     </row>
     <row r="71">
@@ -2417,25 +2417,25 @@
         <v>70</v>
       </c>
       <c r="C71" t="n">
-        <v>2.12</v>
+        <v>2.125</v>
       </c>
       <c r="D71" t="n">
-        <v>0.695</v>
+        <v>0.7</v>
       </c>
       <c r="E71" t="n">
-        <v>0.516</v>
+        <v>0.55</v>
       </c>
       <c r="F71" t="n">
-        <v>0.591</v>
+        <v>0.624</v>
       </c>
       <c r="G71" t="n">
-        <v>0.67</v>
+        <v>0.704</v>
       </c>
       <c r="H71" t="n">
-        <v>0.756</v>
+        <v>0.788</v>
       </c>
       <c r="I71" t="n">
-        <v>1.0065</v>
+        <v>1.01875</v>
       </c>
     </row>
     <row r="72">
@@ -2446,25 +2446,25 @@
         <v>71</v>
       </c>
       <c r="C72" t="n">
-        <v>1.863</v>
+        <v>2.109</v>
       </c>
       <c r="D72" t="n">
-        <v>0.669</v>
+        <v>0.706</v>
       </c>
       <c r="E72" t="n">
-        <v>0.511</v>
+        <v>0.534</v>
       </c>
       <c r="F72" t="n">
-        <v>0.587</v>
+        <v>0.612</v>
       </c>
       <c r="G72" t="n">
-        <v>0.67</v>
+        <v>0.695</v>
       </c>
       <c r="H72" t="n">
-        <v>0.762</v>
+        <v>0.786</v>
       </c>
       <c r="I72" t="n">
-        <v>0.928</v>
+        <v>1.01375</v>
       </c>
     </row>
     <row r="73">
@@ -2475,25 +2475,25 @@
         <v>72</v>
       </c>
       <c r="C73" t="n">
-        <v>1.951</v>
+        <v>1.978</v>
       </c>
       <c r="D73" t="n">
-        <v>0.66</v>
+        <v>0.697</v>
       </c>
       <c r="E73" t="n">
-        <v>0.494</v>
+        <v>0.52</v>
       </c>
       <c r="F73" t="n">
-        <v>0.57</v>
+        <v>0.598</v>
       </c>
       <c r="G73" t="n">
-        <v>0.653</v>
+        <v>0.681</v>
       </c>
       <c r="H73" t="n">
-        <v>0.74</v>
+        <v>0.769</v>
       </c>
       <c r="I73" t="n">
-        <v>0.94125</v>
+        <v>0.973</v>
       </c>
     </row>
     <row r="74">
@@ -2504,25 +2504,25 @@
         <v>73</v>
       </c>
       <c r="C74" t="n">
-        <v>2.07</v>
+        <v>1.868</v>
       </c>
       <c r="D74" t="n">
-        <v>0.676</v>
+        <v>0.677</v>
       </c>
       <c r="E74" t="n">
-        <v>0.506</v>
+        <v>0.502</v>
       </c>
       <c r="F74" t="n">
-        <v>0.587</v>
+        <v>0.582</v>
       </c>
       <c r="G74" t="n">
-        <v>0.671</v>
+        <v>0.665</v>
       </c>
       <c r="H74" t="n">
-        <v>0.758</v>
+        <v>0.754</v>
       </c>
       <c r="I74" t="n">
-        <v>0.982</v>
+        <v>0.931</v>
       </c>
     </row>
     <row r="75">
@@ -2533,25 +2533,25 @@
         <v>74</v>
       </c>
       <c r="C75" t="n">
-        <v>2.138</v>
+        <v>2.087</v>
       </c>
       <c r="D75" t="n">
-        <v>0.695</v>
+        <v>0.696</v>
       </c>
       <c r="E75" t="n">
-        <v>0.534</v>
+        <v>0.52</v>
       </c>
       <c r="F75" t="n">
-        <v>0.613</v>
+        <v>0.598</v>
       </c>
       <c r="G75" t="n">
-        <v>0.6919999999999999</v>
+        <v>0.678</v>
       </c>
       <c r="H75" t="n">
-        <v>0.769</v>
+        <v>0.765</v>
       </c>
       <c r="I75" t="n">
-        <v>1.0155</v>
+        <v>0.99975</v>
       </c>
     </row>
     <row r="76">
@@ -2562,25 +2562,25 @@
         <v>75</v>
       </c>
       <c r="C76" t="n">
-        <v>1.951</v>
+        <v>2.239</v>
       </c>
       <c r="D76" t="n">
-        <v>0.6840000000000001</v>
+        <v>0.722</v>
       </c>
       <c r="E76" t="n">
-        <v>0.521</v>
+        <v>0.5570000000000001</v>
       </c>
       <c r="F76" t="n">
-        <v>0.601</v>
+        <v>0.631</v>
       </c>
       <c r="G76" t="n">
-        <v>0.6820000000000001</v>
+        <v>0.71</v>
       </c>
       <c r="H76" t="n">
-        <v>0.767</v>
+        <v>0.791</v>
       </c>
       <c r="I76" t="n">
-        <v>0.96</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="77">
@@ -2591,25 +2591,25 @@
         <v>76</v>
       </c>
       <c r="C77" t="n">
-        <v>2.137</v>
+        <v>2.089</v>
       </c>
       <c r="D77" t="n">
-        <v>0.701</v>
+        <v>0.702</v>
       </c>
       <c r="E77" t="n">
-        <v>0.539</v>
+        <v>0.532</v>
       </c>
       <c r="F77" t="n">
-        <v>0.611</v>
+        <v>0.61</v>
       </c>
       <c r="G77" t="n">
-        <v>0.6879999999999999</v>
+        <v>0.6929999999999999</v>
       </c>
       <c r="H77" t="n">
-        <v>0.767</v>
+        <v>0.784</v>
       </c>
       <c r="I77" t="n">
-        <v>1.0195</v>
+        <v>1.00625</v>
       </c>
     </row>
     <row r="78">
@@ -2620,25 +2620,25 @@
         <v>77</v>
       </c>
       <c r="C78" t="n">
-        <v>2.175</v>
+        <v>2.032</v>
       </c>
       <c r="D78" t="n">
-        <v>0.6879999999999999</v>
+        <v>0.6909999999999999</v>
       </c>
       <c r="E78" t="n">
-        <v>0.53</v>
+        <v>0.506</v>
       </c>
       <c r="F78" t="n">
-        <v>0.608</v>
+        <v>0.585</v>
       </c>
       <c r="G78" t="n">
-        <v>0.6870000000000001</v>
+        <v>0.669</v>
       </c>
       <c r="H78" t="n">
-        <v>0.769</v>
+        <v>0.761</v>
       </c>
       <c r="I78" t="n">
-        <v>1.02025</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="79">
@@ -2649,25 +2649,25 @@
         <v>78</v>
       </c>
       <c r="C79" t="n">
-        <v>1.958</v>
+        <v>2.049</v>
       </c>
       <c r="D79" t="n">
-        <v>0.678</v>
+        <v>0.6870000000000001</v>
       </c>
       <c r="E79" t="n">
-        <v>0.493</v>
+        <v>0.509</v>
       </c>
       <c r="F79" t="n">
-        <v>0.572</v>
+        <v>0.584</v>
       </c>
       <c r="G79" t="n">
-        <v>0.655</v>
+        <v>0.665</v>
       </c>
       <c r="H79" t="n">
-        <v>0.747</v>
+        <v>0.753</v>
       </c>
       <c r="I79" t="n">
-        <v>0.95175</v>
+        <v>0.983</v>
       </c>
     </row>
     <row r="80">
@@ -2678,25 +2678,25 @@
         <v>79</v>
       </c>
       <c r="C80" t="n">
-        <v>1.848</v>
+        <v>1.961</v>
       </c>
       <c r="D80" t="n">
-        <v>0.667</v>
+        <v>0.673</v>
       </c>
       <c r="E80" t="n">
-        <v>0.482</v>
+        <v>0.467</v>
       </c>
       <c r="F80" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.549</v>
       </c>
       <c r="G80" t="n">
-        <v>0.644</v>
+        <v>0.637</v>
       </c>
       <c r="H80" t="n">
-        <v>0.738</v>
+        <v>0.746</v>
       </c>
       <c r="I80" t="n">
-        <v>0.916</v>
+        <v>0.9435</v>
       </c>
     </row>
     <row r="81">
@@ -2707,25 +2707,25 @@
         <v>8</v>
       </c>
       <c r="C81" t="n">
-        <v>2.133</v>
+        <v>2.411</v>
       </c>
       <c r="D81" t="n">
-        <v>0.65</v>
+        <v>0.705</v>
       </c>
       <c r="E81" t="n">
-        <v>0.5610000000000001</v>
+        <v>0.5629999999999999</v>
       </c>
       <c r="F81" t="n">
-        <v>0.637</v>
+        <v>0.635</v>
       </c>
       <c r="G81" t="n">
-        <v>0.709</v>
+        <v>0.716</v>
       </c>
       <c r="H81" t="n">
-        <v>0.784</v>
+        <v>0.796</v>
       </c>
       <c r="I81" t="n">
-        <v>0.9985000000000001</v>
+        <v>1.096</v>
       </c>
     </row>
     <row r="82">
@@ -2736,25 +2736,25 @@
         <v>80</v>
       </c>
       <c r="C82" t="n">
-        <v>1.852</v>
+        <v>2.085</v>
       </c>
       <c r="D82" t="n">
-        <v>0.647</v>
+        <v>0.695</v>
       </c>
       <c r="E82" t="n">
-        <v>0.459</v>
+        <v>0.534</v>
       </c>
       <c r="F82" t="n">
-        <v>0.539</v>
+        <v>0.606</v>
       </c>
       <c r="G82" t="n">
-        <v>0.625</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="H82" t="n">
-        <v>0.724</v>
+        <v>0.768</v>
       </c>
       <c r="I82" t="n">
-        <v>0.90125</v>
+        <v>1.00225</v>
       </c>
     </row>
     <row r="83">
@@ -2765,25 +2765,25 @@
         <v>81</v>
       </c>
       <c r="C83" t="n">
-        <v>1.895</v>
+        <v>1.828</v>
       </c>
       <c r="D83" t="n">
-        <v>0.659</v>
+        <v>0.681</v>
       </c>
       <c r="E83" t="n">
-        <v>0.464</v>
+        <v>0.526</v>
       </c>
       <c r="F83" t="n">
-        <v>0.546</v>
+        <v>0.606</v>
       </c>
       <c r="G83" t="n">
-        <v>0.631</v>
+        <v>0.6889999999999999</v>
       </c>
       <c r="H83" t="n">
-        <v>0.731</v>
+        <v>0.777</v>
       </c>
       <c r="I83" t="n">
-        <v>0.91925</v>
+        <v>0.929</v>
       </c>
     </row>
     <row r="84">
@@ -2794,25 +2794,25 @@
         <v>82</v>
       </c>
       <c r="C84" t="n">
-        <v>1.801</v>
+        <v>1.779</v>
       </c>
       <c r="D84" t="n">
-        <v>0.65</v>
+        <v>0.6840000000000001</v>
       </c>
       <c r="E84" t="n">
-        <v>0.457</v>
+        <v>0.512</v>
       </c>
       <c r="F84" t="n">
-        <v>0.539</v>
+        <v>0.592</v>
       </c>
       <c r="G84" t="n">
-        <v>0.626</v>
+        <v>0.678</v>
       </c>
       <c r="H84" t="n">
-        <v>0.728</v>
+        <v>0.77</v>
       </c>
       <c r="I84" t="n">
-        <v>0.8895</v>
+        <v>0.91475</v>
       </c>
     </row>
     <row r="85">
@@ -2823,25 +2823,25 @@
         <v>83</v>
       </c>
       <c r="C85" t="n">
-        <v>1.789</v>
+        <v>2.106</v>
       </c>
       <c r="D85" t="n">
-        <v>0.676</v>
+        <v>0.695</v>
       </c>
       <c r="E85" t="n">
-        <v>0.483</v>
+        <v>0.538</v>
       </c>
       <c r="F85" t="n">
-        <v>0.5590000000000001</v>
+        <v>0.611</v>
       </c>
       <c r="G85" t="n">
-        <v>0.64</v>
+        <v>0.6919999999999999</v>
       </c>
       <c r="H85" t="n">
-        <v>0.735</v>
+        <v>0.781</v>
       </c>
       <c r="I85" t="n">
-        <v>0.906</v>
+        <v>1.0085</v>
       </c>
     </row>
     <row r="86">
@@ -2852,25 +2852,25 @@
         <v>84</v>
       </c>
       <c r="C86" t="n">
-        <v>1.932</v>
+        <v>1.897</v>
       </c>
       <c r="D86" t="n">
-        <v>0.6909999999999999</v>
+        <v>0.6860000000000001</v>
       </c>
       <c r="E86" t="n">
-        <v>0.512</v>
+        <v>0.503</v>
       </c>
       <c r="F86" t="n">
-        <v>0.591</v>
+        <v>0.58</v>
       </c>
       <c r="G86" t="n">
-        <v>0.675</v>
+        <v>0.666</v>
       </c>
       <c r="H86" t="n">
-        <v>0.764</v>
+        <v>0.758</v>
       </c>
       <c r="I86" t="n">
-        <v>0.9565</v>
+        <v>0.9429999999999999</v>
       </c>
     </row>
     <row r="87">
@@ -2881,25 +2881,25 @@
         <v>85</v>
       </c>
       <c r="C87" t="n">
-        <v>1.985</v>
+        <v>1.784</v>
       </c>
       <c r="D87" t="n">
-        <v>0.681</v>
+        <v>0.6929999999999999</v>
       </c>
       <c r="E87" t="n">
-        <v>0.497</v>
+        <v>0.507</v>
       </c>
       <c r="F87" t="n">
-        <v>0.576</v>
+        <v>0.588</v>
       </c>
       <c r="G87" t="n">
-        <v>0.661</v>
+        <v>0.676</v>
       </c>
       <c r="H87" t="n">
-        <v>0.756</v>
+        <v>0.77</v>
       </c>
       <c r="I87" t="n">
-        <v>0.961</v>
+        <v>0.91925</v>
       </c>
     </row>
     <row r="88">
@@ -2910,25 +2910,25 @@
         <v>86</v>
       </c>
       <c r="C88" t="n">
-        <v>1.839</v>
+        <v>1.987</v>
       </c>
       <c r="D88" t="n">
-        <v>0.66</v>
+        <v>0.6919999999999999</v>
       </c>
       <c r="E88" t="n">
-        <v>0.482</v>
+        <v>0.522</v>
       </c>
       <c r="F88" t="n">
-        <v>0.5590000000000001</v>
+        <v>0.603</v>
       </c>
       <c r="G88" t="n">
-        <v>0.645</v>
+        <v>0.6889999999999999</v>
       </c>
       <c r="H88" t="n">
-        <v>0.739</v>
+        <v>0.772</v>
       </c>
       <c r="I88" t="n">
-        <v>0.91025</v>
+        <v>0.9732499999999999</v>
       </c>
     </row>
     <row r="89">
@@ -2939,25 +2939,25 @@
         <v>87</v>
       </c>
       <c r="C89" t="n">
-        <v>1.982</v>
+        <v>2.167</v>
       </c>
       <c r="D89" t="n">
-        <v>0.663</v>
+        <v>0.711</v>
       </c>
       <c r="E89" t="n">
-        <v>0.492</v>
+        <v>0.54</v>
       </c>
       <c r="F89" t="n">
-        <v>0.571</v>
+        <v>0.616</v>
       </c>
       <c r="G89" t="n">
-        <v>0.654</v>
+        <v>0.698</v>
       </c>
       <c r="H89" t="n">
-        <v>0.746</v>
+        <v>0.78</v>
       </c>
       <c r="I89" t="n">
-        <v>0.95</v>
+        <v>1.03225</v>
       </c>
     </row>
     <row r="90">
@@ -2968,25 +2968,25 @@
         <v>88</v>
       </c>
       <c r="C90" t="n">
-        <v>1.979</v>
+        <v>2.164</v>
       </c>
       <c r="D90" t="n">
-        <v>0.6850000000000001</v>
+        <v>0.724</v>
       </c>
       <c r="E90" t="n">
-        <v>0.521</v>
+        <v>0.547</v>
       </c>
       <c r="F90" t="n">
-        <v>0.596</v>
+        <v>0.623</v>
       </c>
       <c r="G90" t="n">
-        <v>0.678</v>
+        <v>0.704</v>
       </c>
       <c r="H90" t="n">
-        <v>0.762</v>
+        <v>0.786</v>
       </c>
       <c r="I90" t="n">
-        <v>0.9675</v>
+        <v>1.03975</v>
       </c>
     </row>
     <row r="91">
@@ -2997,25 +2997,25 @@
         <v>89</v>
       </c>
       <c r="C91" t="n">
-        <v>2.008</v>
+        <v>2.221</v>
       </c>
       <c r="D91" t="n">
-        <v>0.679</v>
+        <v>0.714</v>
       </c>
       <c r="E91" t="n">
-        <v>0.509</v>
+        <v>0.546</v>
       </c>
       <c r="F91" t="n">
-        <v>0.586</v>
+        <v>0.628</v>
       </c>
       <c r="G91" t="n">
-        <v>0.67</v>
+        <v>0.712</v>
       </c>
       <c r="H91" t="n">
-        <v>0.758</v>
+        <v>0.793</v>
       </c>
       <c r="I91" t="n">
-        <v>0.96875</v>
+        <v>1.04875</v>
       </c>
     </row>
     <row r="92">
@@ -3026,25 +3026,25 @@
         <v>9</v>
       </c>
       <c r="C92" t="n">
-        <v>2.055</v>
+        <v>2.23</v>
       </c>
       <c r="D92" t="n">
-        <v>0.654</v>
+        <v>0.694</v>
       </c>
       <c r="E92" t="n">
-        <v>0.532</v>
+        <v>0.5659999999999999</v>
       </c>
       <c r="F92" t="n">
-        <v>0.613</v>
+        <v>0.643</v>
       </c>
       <c r="G92" t="n">
-        <v>0.696</v>
+        <v>0.723</v>
       </c>
       <c r="H92" t="n">
-        <v>0.779</v>
+        <v>0.803</v>
       </c>
       <c r="I92" t="n">
-        <v>0.97375</v>
+        <v>1.046</v>
       </c>
     </row>
     <row r="93">
@@ -3055,25 +3055,25 @@
         <v>90</v>
       </c>
       <c r="C93" t="n">
-        <v>2.036</v>
+        <v>1.927</v>
       </c>
       <c r="D93" t="n">
-        <v>0.677</v>
+        <v>0.6850000000000001</v>
       </c>
       <c r="E93" t="n">
-        <v>0.476</v>
+        <v>0.519</v>
       </c>
       <c r="F93" t="n">
-        <v>0.5570000000000001</v>
+        <v>0.597</v>
       </c>
       <c r="G93" t="n">
-        <v>0.642</v>
+        <v>0.681</v>
       </c>
       <c r="H93" t="n">
-        <v>0.744</v>
+        <v>0.769</v>
       </c>
       <c r="I93" t="n">
-        <v>0.9665</v>
+        <v>0.954</v>
       </c>
     </row>
     <row r="94">
@@ -3084,25 +3084,25 @@
         <v>91</v>
       </c>
       <c r="C94" t="n">
-        <v>2.038</v>
+        <v>2.024</v>
       </c>
       <c r="D94" t="n">
-        <v>0.67</v>
+        <v>0.702</v>
       </c>
       <c r="E94" t="n">
-        <v>0.499</v>
+        <v>0.535</v>
       </c>
       <c r="F94" t="n">
-        <v>0.58</v>
+        <v>0.61</v>
       </c>
       <c r="G94" t="n">
-        <v>0.666</v>
+        <v>0.6909999999999999</v>
       </c>
       <c r="H94" t="n">
-        <v>0.758</v>
+        <v>0.774</v>
       </c>
       <c r="I94" t="n">
-        <v>0.9692499999999999</v>
+        <v>0.99075</v>
       </c>
     </row>
     <row r="95">
@@ -3113,25 +3113,25 @@
         <v>92</v>
       </c>
       <c r="C95" t="n">
-        <v>2.053</v>
+        <v>1.898</v>
       </c>
       <c r="D95" t="n">
-        <v>0.664</v>
+        <v>0.669</v>
       </c>
       <c r="E95" t="n">
         <v>0.493</v>
       </c>
       <c r="F95" t="n">
-        <v>0.572</v>
+        <v>0.574</v>
       </c>
       <c r="G95" t="n">
-        <v>0.655</v>
+        <v>0.658</v>
       </c>
       <c r="H95" t="n">
-        <v>0.746</v>
+        <v>0.748</v>
       </c>
       <c r="I95" t="n">
-        <v>0.9685</v>
+        <v>0.93225</v>
       </c>
     </row>
     <row r="96">
@@ -3142,25 +3142,25 @@
         <v>93</v>
       </c>
       <c r="C96" t="n">
-        <v>1.997</v>
+        <v>2.001</v>
       </c>
       <c r="D96" t="n">
-        <v>0.663</v>
+        <v>0.7</v>
       </c>
       <c r="E96" t="n">
-        <v>0.477</v>
+        <v>0.531</v>
       </c>
       <c r="F96" t="n">
-        <v>0.554</v>
+        <v>0.61</v>
       </c>
       <c r="G96" t="n">
-        <v>0.638</v>
+        <v>0.694</v>
       </c>
       <c r="H96" t="n">
-        <v>0.734</v>
+        <v>0.779</v>
       </c>
       <c r="I96" t="n">
-        <v>0.95</v>
+        <v>0.983</v>
       </c>
     </row>
     <row r="97">
@@ -3171,25 +3171,25 @@
         <v>94</v>
       </c>
       <c r="C97" t="n">
-        <v>1.781</v>
+        <v>2.091</v>
       </c>
       <c r="D97" t="n">
-        <v>0.644</v>
+        <v>0.711</v>
       </c>
       <c r="E97" t="n">
-        <v>0.454</v>
+        <v>0.522</v>
       </c>
       <c r="F97" t="n">
-        <v>0.536</v>
+        <v>0.6</v>
       </c>
       <c r="G97" t="n">
-        <v>0.62</v>
+        <v>0.6850000000000001</v>
       </c>
       <c r="H97" t="n">
-        <v>0.723</v>
+        <v>0.773</v>
       </c>
       <c r="I97" t="n">
-        <v>0.88075</v>
+        <v>1.00875</v>
       </c>
     </row>
     <row r="98">
@@ -3200,25 +3200,25 @@
         <v>95</v>
       </c>
       <c r="C98" t="n">
-        <v>1.74</v>
+        <v>2.297</v>
       </c>
       <c r="D98" t="n">
-        <v>0.646</v>
+        <v>0.723</v>
       </c>
       <c r="E98" t="n">
-        <v>0.439</v>
+        <v>0.543</v>
       </c>
       <c r="F98" t="n">
-        <v>0.514</v>
+        <v>0.619</v>
       </c>
       <c r="G98" t="n">
-        <v>0.596</v>
+        <v>0.701</v>
       </c>
       <c r="H98" t="n">
-        <v>0.7</v>
+        <v>0.786</v>
       </c>
       <c r="I98" t="n">
-        <v>0.86775</v>
+        <v>1.0715</v>
       </c>
     </row>
     <row r="99">
@@ -3229,25 +3229,25 @@
         <v>96</v>
       </c>
       <c r="C99" t="n">
-        <v>1.822</v>
+        <v>2.092</v>
       </c>
       <c r="D99" t="n">
-        <v>0.642</v>
+        <v>0.6919999999999999</v>
       </c>
       <c r="E99" t="n">
-        <v>0.46</v>
+        <v>0.502</v>
       </c>
       <c r="F99" t="n">
-        <v>0.545</v>
+        <v>0.584</v>
       </c>
       <c r="G99" t="n">
-        <v>0.631</v>
+        <v>0.67</v>
       </c>
       <c r="H99" t="n">
-        <v>0.728</v>
+        <v>0.757</v>
       </c>
       <c r="I99" t="n">
-        <v>0.8915</v>
+        <v>0.9945000000000001</v>
       </c>
     </row>
     <row r="100">
@@ -3258,25 +3258,25 @@
         <v>97</v>
       </c>
       <c r="C100" t="n">
-        <v>1.834</v>
+        <v>2.137</v>
       </c>
       <c r="D100" t="n">
-        <v>0.659</v>
+        <v>0.718</v>
       </c>
       <c r="E100" t="n">
-        <v>0.497</v>
+        <v>0.536</v>
       </c>
       <c r="F100" t="n">
-        <v>0.577</v>
+        <v>0.61</v>
       </c>
       <c r="G100" t="n">
-        <v>0.662</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="H100" t="n">
-        <v>0.751</v>
+        <v>0.773</v>
       </c>
       <c r="I100" t="n">
-        <v>0.91225</v>
+        <v>1.02725</v>
       </c>
     </row>
     <row r="101">
@@ -3287,25 +3287,25 @@
         <v>98</v>
       </c>
       <c r="C101" t="n">
-        <v>1.9</v>
+        <v>2.026</v>
       </c>
       <c r="D101" t="n">
-        <v>0.659</v>
+        <v>0.7</v>
       </c>
       <c r="E101" t="n">
-        <v>0.484</v>
+        <v>0.524</v>
       </c>
       <c r="F101" t="n">
-        <v>0.5610000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="G101" t="n">
-        <v>0.642</v>
+        <v>0.6830000000000001</v>
       </c>
       <c r="H101" t="n">
-        <v>0.73</v>
+        <v>0.771</v>
       </c>
       <c r="I101" t="n">
-        <v>0.9255</v>
+        <v>0.9875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>